<commit_message>
added datadriven as dynamic methods and Datautil.java file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,80 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspace\projectwork\RestAssuredAPIFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07E77B5-5591-4401-B0D3-136252CDE359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAB6EE9-9F0F-4B48-8A93-16D9A751E751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1569C64B-C231-4506-B54B-7AF690AF8E19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="validateCreateCustomerAPI" sheetId="1" r:id="rId1"/>
-    <sheet name="invalidateCreateCustomerAPI" sheetId="2" r:id="rId2"/>
+    <sheet name="testdata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>validateCreateCustomerAPIWithValidSecretKey</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>Kumar Kishan</t>
   </si>
   <si>
+    <t>#30th main road</t>
+  </si>
+  <si>
+    <t>This is request for kumar customer creation</t>
+  </si>
+  <si>
     <t>kk123@gmail.com</t>
   </si>
   <si>
-    <t>This is request for kumar customer creation</t>
-  </si>
-  <si>
-    <t>#24 main road</t>
-  </si>
-  <si>
     <t>Asif Khan</t>
   </si>
   <si>
+    <t>#31th main road</t>
+  </si>
+  <si>
+    <t>This is request for asif customer creation</t>
+  </si>
+  <si>
     <t>ak123@gmail.com</t>
   </si>
   <si>
-    <t>This is request for asif customer creation</t>
-  </si>
-  <si>
-    <t>#25th main road</t>
+    <t>Maharaj Saxena</t>
+  </si>
+  <si>
+    <t>#32th main road</t>
+  </si>
+  <si>
+    <t>This is request for maharaj customer creation</t>
+  </si>
+  <si>
+    <t>mhrj@gmail.com</t>
+  </si>
+  <si>
+    <t>Kumar rawat</t>
+  </si>
+  <si>
+    <t>#33th main road</t>
+  </si>
+  <si>
+    <t>This is request for rawat customer creation</t>
+  </si>
+  <si>
+    <t>kmr@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,38 +102,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -121,34 +119,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -181,7 +159,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -193,7 +171,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -240,23 +218,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -292,23 +253,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,135 +404,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EE65AD-5240-4067-82F6-0BDE59445D3E}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B533EF57-B78B-4551-A134-B26C819687B1}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{E6634AD3-ECCB-45A0-A618-0F418EDD690C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F706F3A-E747-4332-A97F-70AAD438C8FC}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{27AFB8BB-1104-4663-8750-80858D50DB57}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{9ED95E71-88C6-4747-A692-E61BE7C1E4C1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added suite file (testng.xml) and apply business strategy for maintaining the code.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspace\projectwork\RestAssuredAPIFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAB6EE9-9F0F-4B48-8A93-16D9A751E751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C0AEF6-CCD9-4E39-95D4-78CB750403A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>validateCreateCustomerAPIWithValidSecretKey</t>
   </si>
@@ -88,16 +88,51 @@
   </si>
   <si>
     <t>kmr@gmail.com</t>
+  </si>
+  <si>
+    <t>validateCreateCustomerAPIWithInValidSecretKey</t>
+  </si>
+  <si>
+    <t>Kumar Kishan1</t>
+  </si>
+  <si>
+    <t>Asif Khan1</t>
+  </si>
+  <si>
+    <t>Maharaj Saxena1</t>
+  </si>
+  <si>
+    <t>Kumar rawat1</t>
+  </si>
+  <si>
+    <t>kkinvalid123@gmail.com</t>
+  </si>
+  <si>
+    <t>akinvalid123@gmail.com</t>
+  </si>
+  <si>
+    <t>mhrjinvalid@gmail.com</t>
+  </si>
+  <si>
+    <t>kmrinvalid@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,13 +155,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,18 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -494,7 +532,88 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{6ED5C360-A61C-4C9C-9D95-DAF6CAF77C98}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{1B490331-E603-4E0C-A38D-741536B58C34}"/>
+    <hyperlink ref="D12" r:id="rId3" xr:uid="{2CD4DBBE-08A2-41C4-AFE3-5D6457C5142C}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{D3DF9F92-A097-49A8-A8D7-1427FEAB902A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Deleted Customer files and parallel execution
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspace\projectwork\RestAssuredAPIFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C0AEF6-CCD9-4E39-95D4-78CB750403A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F819B700-3A81-4C72-A112-B5FBEA65ACFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>validateCreateCustomerAPIWithValidSecretKey</t>
   </si>
@@ -115,6 +115,84 @@
   </si>
   <si>
     <t>kmrinvalid@gmail.com</t>
+  </si>
+  <si>
+    <t>deleteCustomer</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>cus_HZ8Ote1YmzICWz</t>
+  </si>
+  <si>
+    <t>cus_HZ8ObxRWGVX1qp</t>
+  </si>
+  <si>
+    <t>cus_HZ8OBhoObtvB01</t>
+  </si>
+  <si>
+    <t>cus_HZ8OsWtTlxTCSX</t>
+  </si>
+  <si>
+    <t>cus_HZ8E8JyQgfXL5P</t>
+  </si>
+  <si>
+    <t>cus_HZ8E8zGCxZJKRp</t>
+  </si>
+  <si>
+    <t>cus_HZ8Ep4qH1GlEJK</t>
+  </si>
+  <si>
+    <t>cus_HZ8EaNUAqF7wpW</t>
+  </si>
+  <si>
+    <t>cus_HZ80EGz3k4lL6w</t>
+  </si>
+  <si>
+    <t>cus_HZ80qDVZGCc6VY</t>
+  </si>
+  <si>
+    <t>cus_HZ800V4o3DbJyD</t>
+  </si>
+  <si>
+    <t>cus_HZ80fUlylqt0rS</t>
+  </si>
+  <si>
+    <t>cus_HZ7xZTfhGdcLPw</t>
+  </si>
+  <si>
+    <t>cus_HZ7xrBtqZp9Urd</t>
+  </si>
+  <si>
+    <t>cus_HZ7xM6AJnkTJni</t>
+  </si>
+  <si>
+    <t>cus_HZ7xBNsfmt62OW</t>
+  </si>
+  <si>
+    <t>cus_HZ7rgb2PdHSaX8</t>
+  </si>
+  <si>
+    <t>cus_HZ7rwSOTq8truh</t>
+  </si>
+  <si>
+    <t>cus_HZ7rmFdOPmft68</t>
+  </si>
+  <si>
+    <t>cus_HZ7rYvGfZnWAIz</t>
+  </si>
+  <si>
+    <t>cus_HZ7m9YCCLewnbD</t>
+  </si>
+  <si>
+    <t>cus_HZ7mSZYVmRqNhT</t>
+  </si>
+  <si>
+    <t>cus_HZ7mqLUErfDEuo</t>
+  </si>
+  <si>
+    <t>cus_HZ7m9HmNuV5p5N</t>
   </si>
 </sst>
 </file>
@@ -443,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,6 +685,136 @@
         <v>29</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{6ED5C360-A61C-4C9C-9D95-DAF6CAF77C98}"/>
@@ -615,5 +823,6 @@
     <hyperlink ref="D13" r:id="rId4" xr:uid="{D3DF9F92-A097-49A8-A8D7-1427FEAB902A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created Paypal APIs and added in framework created testng file for paypal Added Get method for order details
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspace\projectwork\RestAssuredAPIFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146D42C9-A07C-4260-94D3-4217E6356976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B2F2FA-7C78-4018-9B98-8B244EC0A790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>validateCreateCustomerAPIWithValidSecretKey</t>
   </si>
@@ -87,46 +87,43 @@
     <t>id</t>
   </si>
   <si>
-    <t>Kumar Kishan456</t>
-  </si>
-  <si>
-    <t>Asif Khan456</t>
-  </si>
-  <si>
-    <t>Maharaj Saxena456</t>
-  </si>
-  <si>
-    <t>Kumar rawat456</t>
-  </si>
-  <si>
-    <t>cus_HZKJARKi1VLpyL</t>
-  </si>
-  <si>
-    <t>cus_HZKJPXwrPqZbQQ</t>
-  </si>
-  <si>
-    <t>Archana Gupta4561</t>
-  </si>
-  <si>
-    <t>Suman Kumari4561</t>
-  </si>
-  <si>
-    <t>Jyoti Saxena4561</t>
-  </si>
-  <si>
-    <t>Kumar rawat rathode4561</t>
-  </si>
-  <si>
-    <t>ag4561@gmail.com</t>
-  </si>
-  <si>
-    <t>sk4561@gmail.com</t>
-  </si>
-  <si>
-    <t>jsj4561@gmail.com</t>
-  </si>
-  <si>
-    <t>kmrr4561@gmail.com</t>
+    <t>ag12876@gmail.com</t>
+  </si>
+  <si>
+    <t>sk12876@gmail.com</t>
+  </si>
+  <si>
+    <t>jsj12876@gmail.com</t>
+  </si>
+  <si>
+    <t>kmrr12876@gmail.com</t>
+  </si>
+  <si>
+    <t>Kumar Kishan12876</t>
+  </si>
+  <si>
+    <t>Asif Khan12876</t>
+  </si>
+  <si>
+    <t>Maharaj Saxena12876</t>
+  </si>
+  <si>
+    <t>Kumar rawat12876</t>
+  </si>
+  <si>
+    <t>Archana Gupta12877</t>
+  </si>
+  <si>
+    <t>Suman Kumari12877</t>
+  </si>
+  <si>
+    <t>Jyoti Saxena12877</t>
+  </si>
+  <si>
+    <t>Kumar rawat rathode12877</t>
+  </si>
+  <si>
+    <t>cus_Hb286lXLYZuvlx</t>
   </si>
 </sst>
 </file>
@@ -455,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,7 +487,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -499,12 +496,12 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -513,12 +510,12 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -527,12 +524,12 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -541,7 +538,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -565,7 +562,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -579,7 +576,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -593,7 +590,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -607,7 +604,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -631,12 +628,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Update,Retrieve and Retrieve all files
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspace\projectwork\RestAssuredAPIFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998AE52A-5FED-46E8-AFE3-81B0A8BCA9B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E263B518-45D0-4AB5-B8DC-BCA0A4DEC97B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>validateCreateCustomerAPIWithValidSecretKey</t>
   </si>
@@ -87,9 +88,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>cus_Hb286lXLYZuvlx</t>
-  </si>
-  <si>
     <t>updateCustomer</t>
   </si>
   <si>
@@ -105,28 +103,88 @@
     <t>Kumar rawat12877</t>
   </si>
   <si>
-    <t>Archana Gupta12875</t>
-  </si>
-  <si>
-    <t>Suman Kumari12875</t>
-  </si>
-  <si>
-    <t>Jyoti Saxena12875</t>
-  </si>
-  <si>
-    <t>Kumar rawat rathode12875</t>
-  </si>
-  <si>
-    <t>ag12875@gmail.com</t>
-  </si>
-  <si>
-    <t>sk12875@gmail.com</t>
-  </si>
-  <si>
-    <t>jsj12875@gmail.com</t>
-  </si>
-  <si>
-    <t>kmrr12875@gmail.com</t>
+    <t>cus_HgcZz63aVSMVKQ</t>
+  </si>
+  <si>
+    <t>jsj1234@gmail.com</t>
+  </si>
+  <si>
+    <t>Update data</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>getIDCustomerDetails</t>
+  </si>
+  <si>
+    <t>getAllListCustomerDetails</t>
+  </si>
+  <si>
+    <t>Archana Gupta</t>
+  </si>
+  <si>
+    <t>Suman Kumari</t>
+  </si>
+  <si>
+    <t>Jyoti Saxena</t>
+  </si>
+  <si>
+    <t>Kumar rawat rathode</t>
+  </si>
+  <si>
+    <t>agtest123@gmail.com</t>
+  </si>
+  <si>
+    <t>sktest123@gmail.com</t>
+  </si>
+  <si>
+    <t>jsjtest123@gmail.com</t>
+  </si>
+  <si>
+    <t>kmrrtest123@gmail.com</t>
+  </si>
+  <si>
+    <t>cus_Hgchao3iSpHM2d</t>
+  </si>
+  <si>
+    <t>cus_HgchrJyWWW791P</t>
+  </si>
+  <si>
+    <t>cus_Hgch5HkKc1B5qM</t>
+  </si>
+  <si>
+    <t>cus_HgcZaxtScCgzLY</t>
+  </si>
+  <si>
+    <t>cus_HgcZUikpPp8R4d</t>
+  </si>
+  <si>
+    <t>cus_HgcZTDrpMk95ee</t>
+  </si>
+  <si>
+    <t>cus_HgcYXpXiW7tkHs</t>
+  </si>
+  <si>
+    <t>cus_HgcYMmqLxaWlaf</t>
+  </si>
+  <si>
+    <t>cus_HgcYtoxVOO9Qy3</t>
+  </si>
+  <si>
+    <t>Mahaveer swami</t>
+  </si>
+  <si>
+    <t>cus_HgcWaBOKEbToQ9</t>
+  </si>
+  <si>
+    <t>cus_HgcTX2CC7Hxf8G</t>
+  </si>
+  <si>
+    <t>cus_HgcTWeGxbcHnIw</t>
+  </si>
+  <si>
+    <t>cus_HgcTELHZriVt1f</t>
   </si>
 </sst>
 </file>
@@ -158,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -166,14 +224,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,189 +529,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -649,8 +980,26 @@
     <hyperlink ref="D4" r:id="rId6" xr:uid="{E7139462-B194-4E75-BCD6-8CC8419FABA6}"/>
     <hyperlink ref="D5" r:id="rId7" xr:uid="{EF55F763-2B2C-449C-8C26-D1ACE6842278}"/>
     <hyperlink ref="D6" r:id="rId8" xr:uid="{A1884565-7E7C-47BB-912B-9BE267A97639}"/>
+    <hyperlink ref="E30" r:id="rId9" xr:uid="{1864E4B1-3BDF-41D0-BC84-6501B7A1343C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB7098A-AA61-43AC-A188-9277FA54E278}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>